<commit_message>
TRIFFHIR-39: Import value sets from excel files
</commit_message>
<xml_diff>
--- a/test/data/example_vs_import.xlsx
+++ b/test/data/example_vs_import.xlsx
@@ -1,41 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E60CB5-ACB5-4A08-B038-EED311FCEA60}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86923F03-E496-45AB-8425-D39C7CBC990D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Valuesets" sheetId="1" r:id="rId1"/>
-    <sheet name="Concepts" sheetId="2" r:id="rId2"/>
+    <sheet name="Concepts" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Test Valueset 1</t>
-  </si>
-  <si>
-    <t>Test Valueset 2</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
     <t>Display</t>
   </si>
   <si>
-    <t>ValueSet URL</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -45,12 +35,6 @@
     <t>http://test.com/ValueSet/v2</t>
   </si>
   <si>
-    <t>ID (optional)</t>
-  </si>
-  <si>
-    <t>Code System URL</t>
-  </si>
-  <si>
     <t>http://test.com/CodeSystem/cs1</t>
   </si>
   <si>
@@ -67,6 +51,24 @@
   </si>
   <si>
     <t>http://test.com/CodeSystem/cs2</t>
+  </si>
+  <si>
+    <t>Value Set 1</t>
+  </si>
+  <si>
+    <t>Value Set 2</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>vs1-test</t>
+  </si>
+  <si>
+    <t>vs2-test</t>
+  </si>
+  <si>
+    <t>System</t>
   </si>
 </sst>
 </file>
@@ -451,121 +453,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>